<commit_message>
Adding third week logs
</commit_message>
<xml_diff>
--- a/Logs/Opmann_Time_recording_log.xlsx
+++ b/Logs/Opmann_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\source\repos\ISA2\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFDFCE1-79CD-4B63-BDAB-CCDCB4B0EBE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13449B47-287B-4D59-9C0A-E35013D00672}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Regex (Regular Expretions)</t>
+  </si>
+  <si>
+    <t>Node.js</t>
+  </si>
+  <si>
+    <t>ASP.NET MVC Core (Reading and Practising)</t>
   </si>
 </sst>
 </file>
@@ -174,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -492,11 +498,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -607,6 +639,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1780,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE82E465-3E6E-40D2-A181-AF99E900A418}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="46">
-        <v>43506</v>
+        <v>43514</v>
       </c>
       <c r="H4" s="46"/>
       <c r="I4" s="46"/>
@@ -2071,23 +2112,35 @@
       <c r="H13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="33"/>
+      <c r="I13" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="7">
+        <v>43512</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.6875</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.74305555555555547</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="32"/>
+        <v>79.999999999999872</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>36</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="10"/>
     </row>
@@ -2095,16 +2148,22 @@
       <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="7">
+        <v>43513</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5">
         <f>(D15-C15)*24*60 - E15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+        <v>149.99999999999994</v>
+      </c>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="6"/>
       <c r="J15" s="10"/>
     </row>
@@ -2113,36 +2172,54 @@
         <v>10</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="I16" s="6"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>11</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="7">
+        <v>43514</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+        <v>99.999999999999801</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>12</v>
       </c>
@@ -2159,7 +2236,7 @@
       <c r="I18" s="26"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
         <v>14</v>
       </c>
@@ -2169,15 +2246,16 @@
       <c r="E19" s="38"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>544.99999999999977</v>
+        <v>904.99999999999932</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29"/>
+      <c r="O19" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
@@ -2185,6 +2263,8 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Employee to db feature rdy
</commit_message>
<xml_diff>
--- a/Logs/Opmann_Time_recording_log.xlsx
+++ b/Logs/Opmann_Time_recording_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\source\repos\ISA2\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5417CA5-4C2E-44EC-A6DE-4E67374A75B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929DBCE7-9892-4132-A4D6-A1E2C2DBA355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="40">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -542,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -665,6 +665,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2293,7 +2296,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,7 +2502,7 @@
       <c r="G10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="57" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="6"/>
@@ -2509,16 +2512,26 @@
       <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="7">
+        <v>43520</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="57" t="s">
+        <v>38</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -2527,15 +2540,21 @@
         <v>6</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="57" t="s">
+        <v>38</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="10"/>
     </row>
@@ -2653,7 +2672,7 @@
       <c r="E19" s="40"/>
       <c r="F19" s="30">
         <f>SUM(F7:F18)</f>
-        <v>1175.0000000000002</v>
+        <v>1375.0000000000002</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>

</xml_diff>

<commit_message>
6th week logs added
</commit_message>
<xml_diff>
--- a/Logs/Opmann_Time_recording_log.xlsx
+++ b/Logs/Opmann_Time_recording_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\source\repos\ISA2\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D5CC67-3901-4024-9A86-90AACBA6E46F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBC887D-1AF1-45BC-B098-178883ECC849}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Nädal 3" sheetId="4" r:id="rId3"/>
     <sheet name="Nädal 4" sheetId="6" r:id="rId4"/>
     <sheet name="Nädal 5" sheetId="7" r:id="rId5"/>
+    <sheet name="Nädal 6" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="48">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -163,6 +164,21 @@
   </si>
   <si>
     <t>EF Core in an ASP.NET MVC</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Helping other students</t>
+  </si>
+  <si>
+    <t>Teamtreehouse MVC course</t>
+  </si>
+  <si>
+    <t>Teamtreehouse React course</t>
+  </si>
+  <si>
+    <t>Working on my notes</t>
   </si>
 </sst>
 </file>
@@ -2736,7 +2752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15313BE9-DBEA-47E6-9078-AAF43076D9E9}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -3126,4 +3142,408 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BE059D-9677-44C5-834F-8955B1B828D4}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="52">
+        <v>43535</v>
+      </c>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>1</v>
+      </c>
+      <c r="B7" s="38">
+        <v>43532</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21">
+        <f t="shared" ref="F7:F18" si="0">(D7-C7)*24*60 - E7</f>
+        <v>140.00000000000006</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="39">
+        <v>43533</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="6">
+        <v>60</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>35.000000000000036</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
+      <c r="B10" s="39">
+        <v>43534</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>229.99999999999997</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>5</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="8">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>129.99999999999986</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>6</v>
+      </c>
+      <c r="B12" s="39">
+        <v>43535</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>199.99999999999994</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5">
+        <f>(D15-C15)*24*60 - E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
+        <v>12</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="30">
+        <f>SUM(F7:F18)</f>
+        <v>1005</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>